<commit_message>
Atualização automática de SANTA_MARIA.xlsx
</commit_message>
<xml_diff>
--- a/SANTA_MARIA.xlsx
+++ b/SANTA_MARIA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C558121E-FFE8-47A6-BE38-D4775D3C3892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{721E056B-1A2F-4A7D-A740-0902B43FEC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1253,7 +1253,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{2D627B9F-D70E-4BD3-A5E2-DB509BF30735}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{9BF01117-0BAC-4356-945E-8E77E4B1D467}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1283,10 +1283,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{389A45CD-FFE6-4F32-ABBE-57EDEC3178AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B08A8251-9D8A-4E86-BAEB-41AF9D752085}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1324,7 +1324,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEC0ABF3-EE29-45C5-813E-E3628C27DCDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3F81794-42B6-4DAC-96E0-353DC9F8F0F1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1387,7 +1387,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B252D89A-653A-4063-A49E-4D0277197490}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D45EB960-E87A-443C-9B6F-7CFD2BDC7010}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1406,7 +1406,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B765A28-76EB-05DE-E79D-EF3A42609F5C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2FA18A6-F809-F63D-DCA3-1DF38E520EDD}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1455,7 +1455,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F29FE47-B05E-327C-3446-5C9C8AF22139}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{316BD03A-A4F3-35FD-8513-7C008F98AE7D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1474,7 +1474,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F63575B-8E5B-467B-3C60-63C2E00E8B49}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D9409AE-FE12-D99D-F38B-61BD73AF760C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1505,7 +1505,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F85B9752-DEFE-4A04-BD80-4E134C162B1B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{609882D0-8ACD-82A6-586A-D597C7643798}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1536,7 +1536,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3C3AADD-D0DF-0A97-E78E-807E3FF8AC54}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{169E9AAA-B575-EABA-9249-39867560F1E7}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1579,7 +1579,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7137676-E2D5-4F31-AD1F-905D677C3FA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04BB73FF-BC45-4DA3-88A0-7CEE7331A3F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1617,7 +1617,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D775E7F0-ACEA-43C9-A932-3405352A0BBE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BF28248-CECD-4821-900F-42BEA2988A76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1660,7 +1660,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1AD6335-30A1-42D5-AF24-434D1BF1DE02}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{420D76A4-98A0-421E-8E75-AE10A5BCF787}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1973,7 +1973,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD85CEC-3CDA-42EF-9026-58CCB79E5810}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C32428F-7CB8-4375-A1F2-5554DCE104B5}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>